<commit_message>
csv files to use in Plotly.
</commit_message>
<xml_diff>
--- a/FIFA_stats.xlsx
+++ b/FIFA_stats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="-740" windowWidth="24140" windowHeight="17420" tabRatio="500" firstSheet="23" activeTab="27"/>
+    <workbookView xWindow="32240" yWindow="2440" windowWidth="16240" windowHeight="9760" tabRatio="500" firstSheet="22" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="transposed" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="97">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -339,10 +339,6 @@
     <t>Right-back (Full-back)</t>
   </si>
   <si>
-    <t>Goal Keeper</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Center Midfield</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -360,6 +356,10 @@
   </si>
   <si>
     <t>Left Center Back</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Goal Keeper</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -438,7 +438,7 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -463,6 +463,18 @@
         <bgColor indexed="24"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -476,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -501,6 +513,11 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1007,7 +1024,7 @@
         <v>87</v>
       </c>
       <c r="AB2" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AC2" s="13" t="s">
         <v>90</v>
@@ -3596,9 +3613,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H18"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -3607,7 +3622,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -3853,9 +3868,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -3866,7 +3879,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="21" t="s">
         <v>57</v>
       </c>
     </row>
@@ -4115,9 +4128,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H18"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -4127,7 +4138,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="21" t="s">
         <v>61</v>
       </c>
     </row>
@@ -4373,9 +4384,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -4386,7 +4395,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="21" t="s">
         <v>59</v>
       </c>
     </row>
@@ -4630,9 +4639,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H18"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -4643,7 +4650,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="21" t="s">
         <v>63</v>
       </c>
     </row>
@@ -4892,9 +4899,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H18"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -4904,7 +4909,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="21" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5150,9 +5155,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -5162,7 +5165,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="19" t="s">
         <v>69</v>
       </c>
     </row>
@@ -5391,7 +5394,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0" right="0" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5406,11 +5408,9 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H18"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -5420,8 +5420,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>92</v>
+      <c r="A1" s="22" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -5640,34 +5640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18">
-        <v>0.15</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18">
-        <v>0.05</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18">
-        <v>0.1</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18">
-        <v>0.15</v>
-      </c>
-    </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0" right="0" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5684,9 +5657,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -5696,7 +5667,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="19" t="s">
         <v>69</v>
       </c>
     </row>
@@ -5920,7 +5891,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0" right="0" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5937,9 +5907,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H18"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -5951,7 +5919,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="20" t="s">
         <v>73</v>
       </c>
     </row>
@@ -6185,9 +6153,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="137" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView view="pageLayout" zoomScale="137" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -6197,8 +6163,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" t="s">
-        <v>91</v>
+      <c r="A1" s="18" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -6401,7 +6367,6 @@
     </row>
     <row r="22" ht="8" customHeight="1"/>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0" right="0" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6418,9 +6383,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H18"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -6430,7 +6393,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="19" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6671,9 +6634,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H18"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -6683,7 +6644,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="21" t="s">
         <v>79</v>
       </c>
     </row>
@@ -6924,9 +6885,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -6936,7 +6895,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="21" t="s">
         <v>77</v>
       </c>
     </row>
@@ -7195,9 +7154,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H18"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -7207,7 +7164,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="19" t="s">
         <v>81</v>
       </c>
     </row>
@@ -7432,9 +7389,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H18"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -7444,7 +7399,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="21" t="s">
         <v>83</v>
       </c>
     </row>
@@ -7669,9 +7624,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H18"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -7681,8 +7634,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>95</v>
+      <c r="A1" s="22" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -7901,9 +7854,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -7913,8 +7864,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>94</v>
+      <c r="A1" s="22" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -8133,9 +8084,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:H18"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -8144,8 +8093,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>96</v>
+      <c r="A1" s="22" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -8364,9 +8313,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:H18"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -8377,7 +8324,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="19" t="s">
         <v>87</v>
       </c>
     </row>
@@ -8401,7 +8348,7 @@
         <v>12</v>
       </c>
       <c r="F3">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>22</v>
@@ -8427,7 +8374,7 @@
         <v>17</v>
       </c>
       <c r="F4">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>30</v>
@@ -8453,7 +8400,7 @@
         <v>19</v>
       </c>
       <c r="F5">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>39</v>
@@ -8479,7 +8426,7 @@
         <v>21</v>
       </c>
       <c r="F6">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -8613,9 +8560,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:H19"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -8628,7 +8573,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="20" t="s">
         <v>29</v>
       </c>
     </row>
@@ -8879,9 +8824,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -8895,7 +8838,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="21" t="s">
         <v>41</v>
       </c>
     </row>
@@ -9144,7 +9087,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -9161,7 +9104,7 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="20" t="s">
         <v>44</v>
       </c>
     </row>
@@ -9415,9 +9358,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H18"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -9428,7 +9369,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="21" t="s">
         <v>46</v>
       </c>
     </row>
@@ -9677,9 +9618,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -9689,7 +9628,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="21" t="s">
         <v>55</v>
       </c>
     </row>
@@ -9935,9 +9874,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H18"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -9946,7 +9883,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="20" t="s">
         <v>48</v>
       </c>
     </row>
@@ -10198,9 +10135,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -10211,7 +10146,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="21" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>